<commit_message>
Addin comin along, vanilla NN, regression and SVM now working!
</commit_message>
<xml_diff>
--- a/myproject/boston_features.xlsx
+++ b/myproject/boston_features.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://elektaonline-my.sharepoint.com/personal/erik_lagerstroem_elekta_com/Documents/Desktop/git-repo/ExcelPython/myproject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://elektaonline-my.sharepoint.com/personal/erik_lagerstroem_elekta_com/Documents/Desktop/git-repo/ML-addin-excel/myproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_4A4194B38780DE1C9F1B3F11595ED87656C911B4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DF85F4B8-E1EB-4F07-91CB-446593DBB28B}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_4A4194B38780DE1C9F1B3F11595ED87656C911B4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{01866764-91FA-4473-B525-2FCD3719F284}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>